<commit_message>
test set 4 added
</commit_message>
<xml_diff>
--- a/input/calorimetry/test_4.xlsx
+++ b/input/calorimetry/test_4.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KEVreplica\input\calorimetry\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C055BA0D-9908-42C4-AFF3-BAD2C64533F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <sheet name="targets" sheetId="6" r:id="rId6"/>
     <sheet name="enthalpies" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,17 +37,317 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="111">
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>HL</t>
+  </si>
+  <si>
+    <t>H2L</t>
+  </si>
+  <si>
+    <t>HOH</t>
+  </si>
+  <si>
+    <t>HOHD</t>
+  </si>
+  <si>
     <t>lg_k</t>
   </si>
   <si>
     <t>tot</t>
   </si>
   <si>
+    <t>series</t>
+  </si>
+  <si>
+    <t>0.001009623</t>
+  </si>
+  <si>
+    <t>0.000996</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>0.001056023</t>
+  </si>
+  <si>
+    <t>0.000988</t>
+  </si>
+  <si>
+    <t>0.001079035</t>
+  </si>
+  <si>
+    <t>0.000984</t>
+  </si>
+  <si>
+    <t>0.001101954</t>
+  </si>
+  <si>
+    <t>0.00098</t>
+  </si>
+  <si>
+    <t>0.00112478</t>
+  </si>
+  <si>
+    <t>0.000976</t>
+  </si>
+  <si>
+    <t>0.001147514</t>
+  </si>
+  <si>
+    <t>0.000972</t>
+  </si>
+  <si>
+    <t>0.001170156</t>
+  </si>
+  <si>
+    <t>0.000968</t>
+  </si>
+  <si>
+    <t>0.001192706</t>
+  </si>
+  <si>
+    <t>0.000964</t>
+  </si>
+  <si>
+    <t>0.001215164</t>
+  </si>
+  <si>
+    <t>0.00096</t>
+  </si>
+  <si>
+    <t>0.001237532</t>
+  </si>
+  <si>
+    <t>0.000956</t>
+  </si>
+  <si>
+    <t>0.001259809</t>
+  </si>
+  <si>
+    <t>0.000952</t>
+  </si>
+  <si>
+    <t>0.001281996</t>
+  </si>
+  <si>
+    <t>0.000949</t>
+  </si>
+  <si>
+    <t>0.001304093</t>
+  </si>
+  <si>
+    <t>0.000945</t>
+  </si>
+  <si>
+    <t>0.001326101</t>
+  </si>
+  <si>
+    <t>0.000941</t>
+  </si>
+  <si>
+    <t>0.00134802</t>
+  </si>
+  <si>
+    <t>0.000937</t>
+  </si>
+  <si>
+    <t>0.00136985</t>
+  </si>
+  <si>
+    <t>0.000933</t>
+  </si>
+  <si>
+    <t>0.001391591</t>
+  </si>
+  <si>
+    <t>0.00093</t>
+  </si>
+  <si>
+    <t>0.001413245</t>
+  </si>
+  <si>
+    <t>0.000926</t>
+  </si>
+  <si>
+    <t>0.00143481</t>
+  </si>
+  <si>
+    <t>0.000922</t>
+  </si>
+  <si>
+    <t>0.001456289</t>
+  </si>
+  <si>
+    <t>0.000918</t>
+  </si>
+  <si>
+    <t>0.00147768</t>
+  </si>
+  <si>
+    <t>0.000915</t>
+  </si>
+  <si>
+    <t>0.001498985</t>
+  </si>
+  <si>
+    <t>0.000911</t>
+  </si>
+  <si>
+    <t>0.001520204</t>
+  </si>
+  <si>
+    <t>0.000907</t>
+  </si>
+  <si>
+    <t>0.001541337</t>
+  </si>
+  <si>
+    <t>0.000904</t>
+  </si>
+  <si>
+    <t>0.001562384</t>
+  </si>
+  <si>
+    <t>0.0009</t>
+  </si>
+  <si>
+    <t>0.001583346</t>
+  </si>
+  <si>
+    <t>0.000896</t>
+  </si>
+  <si>
+    <t>0.001604223</t>
+  </si>
+  <si>
+    <t>0.000893</t>
+  </si>
+  <si>
+    <t>0.001625016</t>
+  </si>
+  <si>
+    <t>0.000889</t>
+  </si>
+  <si>
+    <t>0.001645724</t>
+  </si>
+  <si>
+    <t>0.000885</t>
+  </si>
+  <si>
+    <t>0.001666349</t>
+  </si>
+  <si>
+    <t>0.000882</t>
+  </si>
+  <si>
+    <t>0.00168689</t>
+  </si>
+  <si>
+    <t>0.000878</t>
+  </si>
+  <si>
+    <t>0.001707348</t>
+  </si>
+  <si>
+    <t>0.000875</t>
+  </si>
+  <si>
+    <t>0.001727723</t>
+  </si>
+  <si>
+    <t>0.000871</t>
+  </si>
+  <si>
+    <t>0.001748016</t>
+  </si>
+  <si>
+    <t>0.000868</t>
+  </si>
+  <si>
+    <t>0.001768226</t>
+  </si>
+  <si>
+    <t>0.000864</t>
+  </si>
+  <si>
+    <t>0.001788355</t>
+  </si>
+  <si>
+    <t>0.000861</t>
+  </si>
+  <si>
+    <t>0.001808402</t>
+  </si>
+  <si>
+    <t>0.000857</t>
+  </si>
+  <si>
+    <t>0.001828368</t>
+  </si>
+  <si>
+    <t>0.000854</t>
+  </si>
+  <si>
+    <t>0.001848253</t>
+  </si>
+  <si>
+    <t>0.00085</t>
+  </si>
+  <si>
+    <t>0.001868058</t>
+  </si>
+  <si>
+    <t>0.000847</t>
+  </si>
+  <si>
+    <t>0.001887782</t>
+  </si>
+  <si>
+    <t>0.000843</t>
+  </si>
+  <si>
+    <t>0.001907427</t>
+  </si>
+  <si>
+    <t>0.00084</t>
+  </si>
+  <si>
+    <t>0.001926992</t>
+  </si>
+  <si>
+    <t>0.000837</t>
+  </si>
+  <si>
+    <t>0.001946478</t>
+  </si>
+  <si>
+    <t>0.000833</t>
+  </si>
+  <si>
+    <t>0.001965885</t>
+  </si>
+  <si>
+    <t>0.00083</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>data</t>
   </si>
   <si>
@@ -69,46 +370,16 @@
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>OH</t>
-  </si>
-  <si>
-    <t>HL</t>
-  </si>
-  <si>
-    <t>H2L</t>
-  </si>
-  <si>
-    <t>HOH</t>
-  </si>
-  <si>
-    <t>HOHD</t>
-  </si>
-  <si>
-    <t>series</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,9 +409,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -420,30 +692,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -454,10 +726,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -468,10 +740,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1</v>
       </c>
@@ -482,10 +754,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>-1</v>
       </c>
@@ -496,7 +768,7 @@
         <v>-1</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -505,36 +777,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5">
         <v>-14</v>
       </c>
@@ -545,917 +817,1557 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AA64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:W1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>9.9799999999999997E-4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>9.9799999999999997E-4</v>
-      </c>
-      <c r="C3">
-        <v>9.9799999999999997E-4</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1.0555350701402805E-3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>9.8800000000000016E-4</v>
-      </c>
-      <c r="C4">
-        <v>9.8800000000000016E-4</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1.0782275449101797E-3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>9.8405588822355304E-4</v>
-      </c>
-      <c r="C5">
-        <v>9.8405588822355304E-4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1.1007395626242546E-3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>9.8014314115308157E-4</v>
-      </c>
-      <c r="C6">
-        <v>9.8014314115308157E-4</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1.1230732673267326E-3</v>
-      </c>
-      <c r="B7" s="1">
-        <v>9.7626138613861389E-4</v>
-      </c>
-      <c r="C7">
-        <v>9.7626138613861389E-4</v>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1.1452307692307693E-3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>9.7241025641025647E-4</v>
-      </c>
-      <c r="C8">
-        <v>9.7241025641025647E-4</v>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1.1672141453831042E-3</v>
-      </c>
-      <c r="B9" s="1">
-        <v>9.6858939096267191E-4</v>
-      </c>
-      <c r="C9">
-        <v>9.6858939096267191E-4</v>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1.1890254403131115E-3</v>
-      </c>
-      <c r="B10" s="1">
-        <v>9.6479843444227014E-4</v>
-      </c>
-      <c r="C10">
-        <v>9.6479843444227014E-4</v>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1.2106666666666667E-3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>9.6103703703703705E-4</v>
-      </c>
-      <c r="C11">
-        <v>9.6103703703703705E-4</v>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1.2321398058252428E-3</v>
-      </c>
-      <c r="B12" s="1">
-        <v>9.5730485436893212E-4</v>
-      </c>
-      <c r="C12">
-        <v>9.5730485436893212E-4</v>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1.2534468085106383E-3</v>
-      </c>
-      <c r="B13" s="1">
-        <v>9.5360154738878143E-4</v>
-      </c>
-      <c r="C13">
-        <v>9.5360154738878143E-4</v>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1.2745895953757227E-3</v>
-      </c>
-      <c r="B14">
-        <v>9.4992678227360313E-4</v>
-      </c>
-      <c r="C14">
-        <v>9.4992678227360313E-4</v>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1.2955700575815739E-3</v>
-      </c>
-      <c r="B15">
-        <v>9.4628023032629566E-4</v>
-      </c>
-      <c r="C15">
-        <v>9.4628023032629566E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1.3163900573613767E-3</v>
-      </c>
-      <c r="B16">
-        <v>9.4266156787762906E-4</v>
-      </c>
-      <c r="C16">
-        <v>9.4266156787762906E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1.3370514285714287E-3</v>
-      </c>
-      <c r="B17">
-        <v>9.3907047619047623E-4</v>
-      </c>
-      <c r="C17">
-        <v>9.3907047619047623E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+    </row>
+    <row r="17" spans="1:25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1.3575559772296014E-3</v>
-      </c>
-      <c r="B18">
-        <v>9.3550664136622392E-4</v>
-      </c>
-      <c r="C18">
-        <v>9.3550664136622392E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+    </row>
+    <row r="18" spans="1:25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1.3779054820415879E-3</v>
-      </c>
-      <c r="B19">
-        <v>9.3196975425330819E-4</v>
-      </c>
-      <c r="C19">
-        <v>9.3196975425330819E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+    </row>
+    <row r="19" spans="1:25">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1.3981016949152541E-3</v>
-      </c>
-      <c r="B20">
-        <v>9.2845951035781544E-4</v>
-      </c>
-      <c r="C20">
-        <v>9.2845951035781544E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1.4181463414634147E-3</v>
-      </c>
-      <c r="B21">
-        <v>9.2497560975609758E-4</v>
-      </c>
-      <c r="C21">
-        <v>9.2497560975609758E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1.4380411214953272E-3</v>
-      </c>
-      <c r="B22">
-        <v>9.2151775700934579E-4</v>
-      </c>
-      <c r="C22">
-        <v>9.2151775700934579E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1.4577877094972067E-3</v>
-      </c>
-      <c r="B23">
-        <v>9.1808566108007449E-4</v>
-      </c>
-      <c r="C23">
-        <v>9.1808566108007449E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1.4773877551020407E-3</v>
-      </c>
-      <c r="B24">
-        <v>9.1467903525046385E-4</v>
-      </c>
-      <c r="C24">
-        <v>9.1467903525046385E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+    </row>
+    <row r="24" spans="1:25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1.4968428835489833E-3</v>
-      </c>
-      <c r="B25">
-        <v>9.1129759704251388E-4</v>
-      </c>
-      <c r="C25">
-        <v>9.1129759704251388E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+    </row>
+    <row r="25" spans="1:25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1.5161546961325967E-3</v>
-      </c>
-      <c r="B26">
-        <v>9.0794106813996318E-4</v>
-      </c>
-      <c r="C26">
-        <v>9.0794106813996318E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+    </row>
+    <row r="26" spans="1:25">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1.5353247706422018E-3</v>
-      </c>
-      <c r="B27">
-        <v>9.0460917431192656E-4</v>
-      </c>
-      <c r="C27">
-        <v>9.0460917431192656E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1.5543546617915905E-3</v>
-      </c>
-      <c r="B28">
-        <v>9.013016453382084E-4</v>
-      </c>
-      <c r="C28">
-        <v>9.013016453382084E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1.5732459016393442E-3</v>
-      </c>
-      <c r="B29">
-        <v>8.9801821493624772E-4</v>
-      </c>
-      <c r="C29">
-        <v>8.9801821493624772E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1.5919999999999999E-3</v>
-      </c>
-      <c r="B30">
-        <v>8.9475862068965511E-4</v>
-      </c>
-      <c r="C30">
-        <v>8.9475862068965511E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+    </row>
+    <row r="30" spans="1:25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1.6106184448462931E-3</v>
-      </c>
-      <c r="B31">
-        <v>8.9152260397830038E-4</v>
-      </c>
-      <c r="C31">
-        <v>8.9152260397830038E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1.629102702702703E-3</v>
-      </c>
-      <c r="B32">
-        <v>8.8830990990991011E-4</v>
-      </c>
-      <c r="C32">
-        <v>8.8830990990991011E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>71</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1.647454219030521E-3</v>
-      </c>
-      <c r="B33">
-        <v>8.8512028725314194E-4</v>
-      </c>
-      <c r="C33">
-        <v>8.8512028725314194E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+    </row>
+    <row r="33" spans="1:25">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
+        <v>73</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1.6656744186046514E-3</v>
-      </c>
-      <c r="B34">
-        <v>8.8195348837209319E-4</v>
-      </c>
-      <c r="C34">
-        <v>8.8195348837209319E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+    </row>
+    <row r="34" spans="1:25">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1.6837647058823531E-3</v>
-      </c>
-      <c r="B35">
-        <v>8.7880926916221046E-4</v>
-      </c>
-      <c r="C35">
-        <v>8.7880926916221046E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+    </row>
+    <row r="35" spans="1:25">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
+        <v>77</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1.7017264653641211E-3</v>
-      </c>
-      <c r="B36">
-        <v>8.7568738898756676E-4</v>
-      </c>
-      <c r="C36">
-        <v>8.7568738898756676E-4</v>
+        <v>13</v>
+      </c>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+    </row>
+    <row r="36" spans="1:25">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1.7195610619469028E-3</v>
-      </c>
-      <c r="B37">
-        <v>8.7258761061946913E-4</v>
-      </c>
-      <c r="C37">
-        <v>8.7258761061946913E-4</v>
+        <v>13</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+    </row>
+    <row r="37" spans="1:25">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" t="s">
+        <v>81</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1.7372698412698416E-3</v>
-      </c>
-      <c r="B38">
-        <v>8.6950970017636694E-4</v>
-      </c>
-      <c r="C38">
-        <v>8.6950970017636694E-4</v>
+        <v>13</v>
+      </c>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+    </row>
+    <row r="38" spans="1:25">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1.7548541300527242E-3</v>
-      </c>
-      <c r="B39">
-        <v>8.6645342706502646E-4</v>
-      </c>
-      <c r="C39">
-        <v>8.6645342706502646E-4</v>
+        <v>13</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+    </row>
+    <row r="39" spans="1:25">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1.7723152364273209E-3</v>
-      </c>
-      <c r="B40">
-        <v>8.6341856392294233E-4</v>
-      </c>
-      <c r="C40">
-        <v>8.6341856392294233E-4</v>
+        <v>13</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+    </row>
+    <row r="40" spans="1:25">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>87</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1.7896544502617802E-3</v>
-      </c>
-      <c r="B41">
-        <v>8.6040488656195476E-4</v>
-      </c>
-      <c r="C41">
-        <v>8.6040488656195476E-4</v>
+        <v>13</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+    </row>
+    <row r="41" spans="1:25">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>89</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>1.8068730434782612E-3</v>
-      </c>
-      <c r="B42">
-        <v>8.5741217391304358E-4</v>
-      </c>
-      <c r="C42">
-        <v>8.5741217391304358E-4</v>
+        <v>13</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41" s="2"/>
+    </row>
+    <row r="42" spans="1:25">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" t="s">
+        <v>91</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1.8239722703639518E-3</v>
-      </c>
-      <c r="B43">
-        <v>8.5444020797227052E-4</v>
-      </c>
-      <c r="C43">
-        <v>8.5444020797227052E-4</v>
+        <v>13</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+    </row>
+    <row r="43" spans="1:25">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" t="s">
+        <v>93</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>1.8409533678756479E-3</v>
-      </c>
-      <c r="B44">
-        <v>8.5148877374784126E-4</v>
-      </c>
-      <c r="C44">
-        <v>8.5148877374784126E-4</v>
+        <v>13</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+    </row>
+    <row r="44" spans="1:25">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" t="s">
+        <v>95</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1.8578175559380379E-3</v>
-      </c>
-      <c r="B45">
-        <v>8.4855765920826176E-4</v>
-      </c>
-      <c r="C45">
-        <v>8.4855765920826176E-4</v>
+        <v>13</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="2"/>
+    </row>
+    <row r="45" spans="1:25">
+      <c r="A45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" t="s">
+        <v>97</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>1.874566037735849E-3</v>
-      </c>
-      <c r="B46">
-        <v>8.4564665523156099E-4</v>
-      </c>
-      <c r="C46">
-        <v>8.4564665523156099E-4</v>
+        <v>13</v>
+      </c>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="2"/>
+    </row>
+    <row r="46" spans="1:25">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" t="s">
+        <v>99</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>1.8912000000000002E-3</v>
-      </c>
-      <c r="B47">
-        <v>8.4275555555555571E-4</v>
-      </c>
-      <c r="C47">
-        <v>8.4275555555555571E-4</v>
+        <v>13</v>
+      </c>
+      <c r="K46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+    </row>
+    <row r="47" spans="1:25">
+      <c r="A47" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" t="s">
+        <v>101</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="K47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+    </row>
+    <row r="48" spans="1:25">
       <c r="A48">
-        <v>1.047E-3</v>
+        <v>1.0854879999999999E-3</v>
       </c>
       <c r="B48">
-        <v>1.047E-3</v>
+        <v>1.0449999999999999E-3</v>
       </c>
       <c r="C48">
-        <v>9.9999999999999998E-17</v>
+        <v>9.9599999999999992E-4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="T48" s="2"/>
+    </row>
+    <row r="49" spans="1:20">
       <c r="A49">
-        <v>1.1997148594377509E-3</v>
+        <v>1.2391279999999999E-3</v>
       </c>
       <c r="B49">
-        <v>1.0385903614457831E-3</v>
+        <v>1.036E-3</v>
       </c>
       <c r="C49">
-        <v>9.9999999999999998E-17</v>
+        <v>9.8799999999999995E-4</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="T49" s="2"/>
+    </row>
+    <row r="50" spans="1:20">
       <c r="A50">
-        <v>1.4795410484668644E-3</v>
+        <v>1.52487E-3</v>
       </c>
       <c r="B50">
-        <v>1.0231810089020772E-3</v>
+        <v>1.021E-3</v>
       </c>
       <c r="C50">
-        <v>9.9999999999999998E-17</v>
+        <v>9.8400000000000007E-4</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="T50" s="2"/>
+    </row>
+    <row r="51" spans="1:20">
       <c r="A51">
-        <v>1.751185185185185E-3</v>
+        <v>1.8062729999999999E-3</v>
       </c>
       <c r="B51">
-        <v>1.0082222222222222E-3</v>
+        <v>1.005E-3</v>
       </c>
       <c r="C51">
-        <v>9.9999999999999998E-17</v>
+        <v>9.7999999999999997E-4</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="T51" s="2"/>
+    </row>
+    <row r="52" spans="1:20">
       <c r="A52">
-        <v>2.0150009606147937E-3</v>
+        <v>2.083405E-3</v>
       </c>
       <c r="B52">
-        <v>9.9369452449567719E-4</v>
+        <v>9.8999999999999999E-4</v>
       </c>
       <c r="C52">
-        <v>9.9999999999999998E-17</v>
+        <v>9.7599999999999998E-4</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="T52" s="2"/>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53">
-        <v>2.2713219696969696E-3</v>
+        <v>2.3563289999999999E-3</v>
       </c>
       <c r="B53">
-        <v>9.7957954545454542E-4</v>
+        <v>9.7499999999999996E-4</v>
       </c>
       <c r="C53">
-        <v>9.9999999999999998E-17</v>
+        <v>9.7199999999999999E-4</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="T53" s="2"/>
+    </row>
+    <row r="54" spans="1:20">
       <c r="A54">
-        <v>2.520463118580766E-3</v>
+        <v>2.625109E-3</v>
       </c>
       <c r="B54">
-        <v>9.6585994397759098E-4</v>
+        <v>9.6000000000000002E-4</v>
       </c>
       <c r="C54">
-        <v>9.9999999999999998E-17</v>
+        <v>9.68E-4</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="T54" s="2"/>
+    </row>
+    <row r="55" spans="1:20">
       <c r="A55">
-        <v>2.7627219152854513E-3</v>
+        <v>2.8898090000000001E-3</v>
       </c>
       <c r="B55">
-        <v>9.5251933701657446E-4</v>
+        <v>9.4600000000000001E-4</v>
       </c>
       <c r="C55">
-        <v>9.9999999999999998E-17</v>
+        <v>9.6400000000000001E-4</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="T55" s="2"/>
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56">
-        <v>2.9983796548592192E-3</v>
+        <v>3.1504900000000001E-3</v>
       </c>
       <c r="B56">
-        <v>9.3954223433242502E-4</v>
+        <v>9.3099999999999997E-4</v>
       </c>
       <c r="C56">
-        <v>9.9999999999999998E-17</v>
+        <v>9.6000000000000002E-4</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="T56" s="2"/>
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57">
-        <v>3.2277025089605732E-3</v>
+        <v>3.4072130000000001E-3</v>
       </c>
       <c r="B57">
-        <v>9.2691397849462346E-4</v>
+        <v>9.1699999999999995E-4</v>
       </c>
       <c r="C57">
-        <v>9.9999999999999998E-17</v>
+        <v>9.5600000000000004E-4</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="T57" s="2"/>
+    </row>
+    <row r="58" spans="1:20">
       <c r="A58">
-        <v>3.4509425287356319E-3</v>
+        <v>3.6600389999999999E-3</v>
       </c>
       <c r="B58">
-        <v>9.1462068965517237E-4</v>
+        <v>9.0300000000000005E-4</v>
       </c>
       <c r="C58">
-        <v>9.9999999999999998E-17</v>
+        <v>9.5200000000000005E-4</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="T58" s="2"/>
+    </row>
+    <row r="59" spans="1:20">
       <c r="A59">
-        <v>3.668338568935428E-3</v>
+        <v>3.9090260000000003E-3</v>
       </c>
       <c r="B59">
-        <v>9.026492146596858E-4</v>
+        <v>8.8900000000000003E-4</v>
       </c>
       <c r="C59">
-        <v>9.9999999999999998E-17</v>
+        <v>9.4899999999999997E-4</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="T59" s="2"/>
+    </row>
+    <row r="60" spans="1:20">
       <c r="A60">
-        <v>3.8801171403962101E-3</v>
+        <v>4.1542339999999997E-3</v>
       </c>
       <c r="B60">
-        <v>8.9098708010335904E-4</v>
+        <v>8.7600000000000004E-4</v>
       </c>
       <c r="C60">
-        <v>9.9999999999999998E-17</v>
+        <v>9.4499999999999998E-4</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="Q60" s="2"/>
+      <c r="T60" s="2"/>
+    </row>
+    <row r="61" spans="1:20">
       <c r="A61">
-        <v>4.086493197278912E-3</v>
+        <v>4.3957179999999998E-3</v>
       </c>
       <c r="B61">
-        <v>8.7962244897959183E-4</v>
+        <v>8.6300000000000005E-4</v>
       </c>
       <c r="C61">
-        <v>9.9999999999999998E-17</v>
+        <v>9.41E-4</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="Q61" s="2"/>
+      <c r="T61" s="2"/>
+    </row>
+    <row r="62" spans="1:20">
       <c r="A62">
-        <v>4.2876708648194794E-3</v>
+        <v>4.6335359999999997E-3</v>
       </c>
       <c r="B62">
-        <v>8.6854408060453385E-4</v>
+        <v>8.4900000000000004E-4</v>
       </c>
       <c r="C62">
-        <v>9.9999999999999998E-17</v>
+        <v>9.3700000000000001E-4</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="Q62" s="2"/>
+      <c r="T62" s="2"/>
+    </row>
+    <row r="63" spans="1:20">
       <c r="A63">
-        <v>4.4838441127694863E-3</v>
+        <v>4.8677429999999999E-3</v>
       </c>
       <c r="B63">
-        <v>8.5774129353233827E-4</v>
+        <v>8.3699999999999996E-4</v>
       </c>
       <c r="C63">
-        <v>9.9999999999999998E-17</v>
+        <v>9.3300000000000002E-4</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20">
       <c r="A64">
-        <v>4.6751973791973791E-3</v>
+        <v>5.0983950000000004E-3</v>
       </c>
       <c r="B64">
-        <v>8.4720393120393106E-4</v>
+        <v>8.2399999999999997E-4</v>
       </c>
       <c r="C64">
-        <v>9.9999999999999998E-17</v>
+        <v>9.3000000000000005E-4</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1464,18 +2376,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1484,18 +2396,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BI5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="AQ17" workbookViewId="0">
       <selection activeCell="BI17" sqref="BI17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1678,9 +2590,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="B2">
         <v>0.998</v>
@@ -1863,9 +2775,9 @@
         <v>1.2210000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="B3">
         <v>3.19E-4</v>
@@ -2048,9 +2960,9 @@
         <v>3.8000000000000002E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2233,9 +3145,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="B5">
         <v>1.0000000000000001E-9</v>
@@ -2425,24 +3337,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2451,34 +3363,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>-55.81</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>55.81</v>

</xml_diff>